<commit_message>
behave et dtcps extraction
</commit_message>
<xml_diff>
--- a/Datasets/DTCPS/DTCPS_pre-extract.xlsx
+++ b/Datasets/DTCPS/DTCPS_pre-extract.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W455"/>
+  <dimension ref="A1:X455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,6 +548,11 @@
           <t>publisher</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>metadata_missing</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -623,6 +628,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -694,6 +700,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -767,6 +774,7 @@
           <t>Elsevier BV</t>
         </is>
       </c>
+      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -838,6 +846,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -913,6 +922,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -984,6 +994,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1059,6 +1070,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1130,6 +1142,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1201,6 +1214,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1272,6 +1286,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1347,6 +1362,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1422,6 +1438,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1497,6 +1514,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1572,6 +1590,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1647,6 +1666,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1718,6 +1738,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1789,6 +1810,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1850,6 +1872,7 @@
         </is>
       </c>
       <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1921,6 +1944,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1992,6 +2016,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2067,6 +2092,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2142,6 +2168,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2213,6 +2240,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2284,6 +2312,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2351,6 +2380,7 @@
         </is>
       </c>
       <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2422,6 +2452,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2493,6 +2524,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2568,6 +2600,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2643,6 +2676,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2714,6 +2748,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2789,6 +2824,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2864,6 +2900,7 @@
           <t>Elsevier Inc.</t>
         </is>
       </c>
+      <c r="X33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2939,6 +2976,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3014,6 +3052,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3089,6 +3128,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3164,6 +3204,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3239,6 +3280,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3310,6 +3352,7 @@
         </is>
       </c>
       <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3385,6 +3428,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3456,6 +3500,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3531,6 +3576,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3606,6 +3652,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3677,6 +3724,7 @@
         </is>
       </c>
       <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3752,6 +3800,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -3827,6 +3876,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -3902,6 +3952,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -3967,6 +4018,7 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr"/>
       <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4038,6 +4090,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4109,6 +4162,7 @@
         </is>
       </c>
       <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4184,6 +4238,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4259,6 +4314,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4334,6 +4390,7 @@
           <t>Elsevier Ltd</t>
         </is>
       </c>
+      <c r="X53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4409,6 +4466,7 @@
           <t>Springer Science and Business Media B.V.</t>
         </is>
       </c>
+      <c r="X54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -4480,6 +4538,7 @@
           <t>Academic Press</t>
         </is>
       </c>
+      <c r="X55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -4555,6 +4614,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -4630,6 +4690,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -4705,6 +4766,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -4780,6 +4842,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -4855,6 +4918,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -4926,6 +4990,7 @@
         </is>
       </c>
       <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5001,6 +5066,7 @@
           <t>Elsevier BV</t>
         </is>
       </c>
+      <c r="X62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5076,6 +5142,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5151,6 +5218,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5226,6 +5294,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5301,6 +5370,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -5376,6 +5446,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -5451,6 +5522,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -5522,6 +5594,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -5597,6 +5670,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -5668,6 +5742,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -5739,6 +5814,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -5810,6 +5886,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -5885,6 +5962,7 @@
           <t>SAGE Publications Ltd</t>
         </is>
       </c>
+      <c r="X74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -5956,6 +6034,7 @@
           <t>MDPI</t>
         </is>
       </c>
+      <c r="X75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6025,6 +6104,7 @@
         </is>
       </c>
       <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6096,6 +6176,7 @@
           <t>Institute of Physics Publishing</t>
         </is>
       </c>
+      <c r="X77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6167,6 +6248,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -6238,6 +6320,7 @@
           <t>MDPI Multidisciplinary Digital Publishing Institute</t>
         </is>
       </c>
+      <c r="X79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -6313,6 +6396,7 @@
           <t>JVE International</t>
         </is>
       </c>
+      <c r="X80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -6384,6 +6468,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -6439,6 +6524,7 @@
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
       <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -6488,6 +6574,7 @@
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr"/>
       <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -6559,6 +6646,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -6630,6 +6718,7 @@
           <t>Hindawi Limited</t>
         </is>
       </c>
+      <c r="X85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -6703,6 +6792,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -6774,6 +6864,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -6845,6 +6936,7 @@
           <t>Hindawi Limited</t>
         </is>
       </c>
+      <c r="X88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -6916,6 +7008,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -6987,6 +7080,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -7058,6 +7152,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -7133,6 +7228,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -7208,6 +7304,7 @@
           <t>Springer Science and Business Media B.V.</t>
         </is>
       </c>
+      <c r="X93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -7283,6 +7380,7 @@
           <t>Wit Press</t>
         </is>
       </c>
+      <c r="X94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -7358,6 +7456,7 @@
           <t>ITMO University</t>
         </is>
       </c>
+      <c r="X95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -7433,6 +7532,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -7508,6 +7608,7 @@
           <t>De Gruyter Open Ltd</t>
         </is>
       </c>
+      <c r="X97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -7579,6 +7680,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -7654,6 +7756,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -7729,6 +7832,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -7800,6 +7904,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -7875,6 +7980,7 @@
           <t>Budapest University of Technology and Economics</t>
         </is>
       </c>
+      <c r="X102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -7946,6 +8052,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -8021,6 +8128,7 @@
           <t>Springer Verlag</t>
         </is>
       </c>
+      <c r="X104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -8092,6 +8200,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -8167,6 +8276,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -8242,6 +8352,7 @@
           <t>Assoc. of Mechanical Eng. and Technicians of Slovenia</t>
         </is>
       </c>
+      <c r="X107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -8313,6 +8424,7 @@
           <t>Hindawi Limited</t>
         </is>
       </c>
+      <c r="X108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -8384,6 +8496,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -8455,6 +8568,7 @@
           <t>MDPI</t>
         </is>
       </c>
+      <c r="X110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -8530,6 +8644,7 @@
           <t>Springer International Publishing</t>
         </is>
       </c>
+      <c r="X111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -8601,6 +8716,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -8672,6 +8788,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -8747,6 +8864,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -8818,6 +8936,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -8893,6 +9012,7 @@
           <t>Springer International Publishing</t>
         </is>
       </c>
+      <c r="X116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -8968,6 +9088,7 @@
           <t>Springer Science and Business Media Deutschland GmbH</t>
         </is>
       </c>
+      <c r="X117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -9021,6 +9142,7 @@
       <c r="U118" t="inlineStr"/>
       <c r="V118" t="inlineStr"/>
       <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -9092,6 +9214,7 @@
           <t>Institute of Physics Publishing</t>
         </is>
       </c>
+      <c r="X119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -9163,6 +9286,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -9238,6 +9362,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -9309,6 +9434,7 @@
           <t>EDP Sciences</t>
         </is>
       </c>
+      <c r="X122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -9380,6 +9506,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -9455,6 +9582,7 @@
           <t>Springer Verlag</t>
         </is>
       </c>
+      <c r="X124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -9530,6 +9658,7 @@
           <t>Springer</t>
         </is>
       </c>
+      <c r="X125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -9605,6 +9734,7 @@
           <t>Springer Verlag</t>
         </is>
       </c>
+      <c r="X126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -9674,6 +9804,7 @@
           <t>SPIE-Intl Soc Optical Eng</t>
         </is>
       </c>
+      <c r="X127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -9745,6 +9876,7 @@
           <t>IOP Publishing Ltd</t>
         </is>
       </c>
+      <c r="X128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -9820,6 +9952,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -9895,6 +10028,7 @@
           <t>MDPI AG</t>
         </is>
       </c>
+      <c r="X130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -9970,6 +10104,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -10025,6 +10160,7 @@
       <c r="U132" t="inlineStr"/>
       <c r="V132" t="inlineStr"/>
       <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -10100,6 +10236,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -10175,6 +10312,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -10250,6 +10388,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -10321,6 +10460,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -10392,6 +10532,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -10463,6 +10604,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -10534,6 +10676,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -10609,6 +10752,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -10662,6 +10806,7 @@
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr"/>
       <c r="W141" t="inlineStr"/>
+      <c r="X141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -10737,6 +10882,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -10808,6 +10954,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -10879,6 +11026,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -10954,6 +11102,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -11017,6 +11166,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -11070,6 +11220,7 @@
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr"/>
       <c r="W147" t="inlineStr"/>
+      <c r="X147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -11145,6 +11296,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -11220,6 +11372,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -11279,6 +11432,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -11354,6 +11508,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -11425,6 +11580,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -11500,6 +11656,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -11573,6 +11730,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -11646,6 +11804,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -11717,6 +11876,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -11792,6 +11952,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -11867,6 +12028,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -11942,6 +12104,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -12021,6 +12184,7 @@
           <t>ACM</t>
         </is>
       </c>
+      <c r="X160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -12090,6 +12254,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -12161,6 +12326,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -12236,6 +12402,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -12315,6 +12482,7 @@
           <t>ACM</t>
         </is>
       </c>
+      <c r="X164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -12386,6 +12554,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -12457,6 +12626,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -12530,6 +12700,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -12601,6 +12772,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -12672,6 +12844,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -12747,6 +12920,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -12818,6 +12992,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -12889,6 +13064,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -12964,6 +13140,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -13039,6 +13216,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -13092,6 +13270,7 @@
       <c r="U175" t="inlineStr"/>
       <c r="V175" t="inlineStr"/>
       <c r="W175" t="inlineStr"/>
+      <c r="X175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -13167,6 +13346,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -13246,6 +13426,7 @@
           <t>ACM</t>
         </is>
       </c>
+      <c r="X177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -13317,6 +13498,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -13392,6 +13574,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -13463,6 +13646,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -13536,6 +13720,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -13611,6 +13796,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -13682,6 +13868,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -13757,6 +13944,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -13832,6 +14020,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -13907,6 +14096,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -13980,6 +14170,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -14055,6 +14246,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -14126,6 +14318,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -14197,6 +14390,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -14272,6 +14466,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -14343,6 +14538,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -14418,6 +14614,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -14493,6 +14690,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -14568,6 +14766,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -14643,6 +14842,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -14718,6 +14918,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -14789,6 +14990,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -14864,6 +15066,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -14939,6 +15142,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -15014,6 +15218,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -15083,6 +15288,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -15158,6 +15364,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -15233,6 +15440,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -15308,6 +15516,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -15383,6 +15592,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -15440,6 +15650,7 @@
         </is>
       </c>
       <c r="W207" t="inlineStr"/>
+      <c r="X207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -15493,6 +15704,7 @@
       <c r="U208" t="inlineStr"/>
       <c r="V208" t="inlineStr"/>
       <c r="W208" t="inlineStr"/>
+      <c r="X208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -15550,6 +15762,7 @@
         </is>
       </c>
       <c r="W209" t="inlineStr"/>
+      <c r="X209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -15605,6 +15818,7 @@
       <c r="U210" t="inlineStr"/>
       <c r="V210" t="inlineStr"/>
       <c r="W210" t="inlineStr"/>
+      <c r="X210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -15676,6 +15890,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -15747,6 +15962,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -15818,6 +16034,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -15891,6 +16108,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -15966,6 +16184,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -16041,6 +16260,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -16114,6 +16334,7 @@
           <t>Association for Computing Machinery (ACM)</t>
         </is>
       </c>
+      <c r="X217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -16173,6 +16394,7 @@
           <t>EDA Consortium</t>
         </is>
       </c>
+      <c r="X218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -16244,6 +16466,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -16315,6 +16538,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -16386,6 +16610,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -16461,6 +16686,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -16532,6 +16758,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -16585,6 +16812,7 @@
       <c r="U224" t="inlineStr"/>
       <c r="V224" t="inlineStr"/>
       <c r="W224" t="inlineStr"/>
+      <c r="X224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -16638,6 +16866,7 @@
       <c r="U225" t="inlineStr"/>
       <c r="V225" t="inlineStr"/>
       <c r="W225" t="inlineStr"/>
+      <c r="X225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -16691,6 +16920,7 @@
       <c r="U226" t="inlineStr"/>
       <c r="V226" t="inlineStr"/>
       <c r="W226" t="inlineStr"/>
+      <c r="X226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -16744,6 +16974,7 @@
       <c r="U227" t="inlineStr"/>
       <c r="V227" t="inlineStr"/>
       <c r="W227" t="inlineStr"/>
+      <c r="X227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -16797,6 +17028,7 @@
       <c r="U228" t="inlineStr"/>
       <c r="V228" t="inlineStr"/>
       <c r="W228" t="inlineStr"/>
+      <c r="X228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -16850,6 +17082,7 @@
       <c r="U229" t="inlineStr"/>
       <c r="V229" t="inlineStr"/>
       <c r="W229" t="inlineStr"/>
+      <c r="X229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -16903,6 +17136,7 @@
       <c r="U230" t="inlineStr"/>
       <c r="V230" t="inlineStr"/>
       <c r="W230" t="inlineStr"/>
+      <c r="X230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -16956,6 +17190,7 @@
       <c r="U231" t="inlineStr"/>
       <c r="V231" t="inlineStr"/>
       <c r="W231" t="inlineStr"/>
+      <c r="X231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -17019,6 +17254,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -17072,6 +17308,7 @@
       <c r="U233" t="inlineStr"/>
       <c r="V233" t="inlineStr"/>
       <c r="W233" t="inlineStr"/>
+      <c r="X233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -17125,6 +17362,7 @@
       <c r="U234" t="inlineStr"/>
       <c r="V234" t="inlineStr"/>
       <c r="W234" t="inlineStr"/>
+      <c r="X234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -17200,6 +17438,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -17255,6 +17494,7 @@
       <c r="U236" t="inlineStr"/>
       <c r="V236" t="inlineStr"/>
       <c r="W236" t="inlineStr"/>
+      <c r="X236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -17326,6 +17566,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -17401,6 +17642,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -17476,6 +17718,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -17551,6 +17794,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -17622,6 +17866,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -17697,6 +17942,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -17768,6 +18014,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -17843,6 +18090,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -17914,6 +18162,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -17989,6 +18238,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -18060,6 +18310,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -18127,6 +18378,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -18200,6 +18452,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -18261,6 +18514,7 @@
         </is>
       </c>
       <c r="W250" t="inlineStr"/>
+      <c r="X250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -18332,6 +18586,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -18403,6 +18658,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -18474,6 +18730,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -18549,6 +18806,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -18620,6 +18878,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -18695,6 +18954,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -18770,6 +19030,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -18845,6 +19106,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -18920,6 +19182,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -18995,6 +19258,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -19066,6 +19330,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -19141,6 +19406,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -19212,6 +19478,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -19283,6 +19550,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -19358,6 +19626,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -19413,6 +19682,7 @@
       <c r="U266" t="inlineStr"/>
       <c r="V266" t="inlineStr"/>
       <c r="W266" t="inlineStr"/>
+      <c r="X266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -19488,6 +19758,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -19543,6 +19814,7 @@
       <c r="U268" t="inlineStr"/>
       <c r="V268" t="inlineStr"/>
       <c r="W268" t="inlineStr"/>
+      <c r="X268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -19614,6 +19886,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -19689,6 +19962,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -19744,6 +20018,7 @@
       <c r="U271" t="inlineStr"/>
       <c r="V271" t="inlineStr"/>
       <c r="W271" t="inlineStr"/>
+      <c r="X271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -19799,6 +20074,7 @@
       <c r="U272" t="inlineStr"/>
       <c r="V272" t="inlineStr"/>
       <c r="W272" t="inlineStr"/>
+      <c r="X272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -19854,6 +20130,7 @@
       <c r="U273" t="inlineStr"/>
       <c r="V273" t="inlineStr"/>
       <c r="W273" t="inlineStr"/>
+      <c r="X273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -19929,6 +20206,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -20004,6 +20282,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -20079,6 +20358,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -20150,6 +20430,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -20225,6 +20506,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -20300,6 +20582,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -20375,6 +20658,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -20450,6 +20734,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -20521,6 +20806,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -20596,6 +20882,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -20667,6 +20954,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -20742,6 +21030,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -20815,6 +21104,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -20890,6 +21180,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -20965,6 +21256,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -21036,6 +21328,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -21095,6 +21388,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -21170,6 +21464,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -21223,6 +21518,7 @@
       <c r="U292" t="inlineStr"/>
       <c r="V292" t="inlineStr"/>
       <c r="W292" t="inlineStr"/>
+      <c r="X292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -21294,6 +21590,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -21347,6 +21644,7 @@
       <c r="U294" t="inlineStr"/>
       <c r="V294" t="inlineStr"/>
       <c r="W294" t="inlineStr"/>
+      <c r="X294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -21400,6 +21698,7 @@
       <c r="U295" t="inlineStr"/>
       <c r="V295" t="inlineStr"/>
       <c r="W295" t="inlineStr"/>
+      <c r="X295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -21453,6 +21752,7 @@
       <c r="U296" t="inlineStr"/>
       <c r="V296" t="inlineStr"/>
       <c r="W296" t="inlineStr"/>
+      <c r="X296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -21506,6 +21806,7 @@
       <c r="U297" t="inlineStr"/>
       <c r="V297" t="inlineStr"/>
       <c r="W297" t="inlineStr"/>
+      <c r="X297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -21559,6 +21860,7 @@
       <c r="U298" t="inlineStr"/>
       <c r="V298" t="inlineStr"/>
       <c r="W298" t="inlineStr"/>
+      <c r="X298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -21612,6 +21914,7 @@
       <c r="U299" t="inlineStr"/>
       <c r="V299" t="inlineStr"/>
       <c r="W299" t="inlineStr"/>
+      <c r="X299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -21687,6 +21990,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -21740,6 +22044,7 @@
       <c r="U301" t="inlineStr"/>
       <c r="V301" t="inlineStr"/>
       <c r="W301" t="inlineStr"/>
+      <c r="X301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -21793,6 +22098,7 @@
       <c r="U302" t="inlineStr"/>
       <c r="V302" t="inlineStr"/>
       <c r="W302" t="inlineStr"/>
+      <c r="X302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -21868,6 +22174,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -21943,6 +22250,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -22018,6 +22326,7 @@
           <t>ICST</t>
         </is>
       </c>
+      <c r="X305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -22091,6 +22400,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -22166,6 +22476,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -22241,6 +22552,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -22312,6 +22624,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -22387,6 +22700,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -22462,6 +22776,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -22533,6 +22848,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -22604,6 +22920,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -22661,6 +22978,7 @@
       <c r="U314" t="inlineStr"/>
       <c r="V314" t="inlineStr"/>
       <c r="W314" t="inlineStr"/>
+      <c r="X314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -22732,6 +23050,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -22785,6 +23104,7 @@
       <c r="U316" t="inlineStr"/>
       <c r="V316" t="inlineStr"/>
       <c r="W316" t="inlineStr"/>
+      <c r="X316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -22860,6 +23180,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -22913,6 +23234,7 @@
       <c r="U318" t="inlineStr"/>
       <c r="V318" t="inlineStr"/>
       <c r="W318" t="inlineStr"/>
+      <c r="X318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -22966,6 +23288,7 @@
       <c r="U319" t="inlineStr"/>
       <c r="V319" t="inlineStr"/>
       <c r="W319" t="inlineStr"/>
+      <c r="X319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -23021,6 +23344,7 @@
       <c r="U320" t="inlineStr"/>
       <c r="V320" t="inlineStr"/>
       <c r="W320" t="inlineStr"/>
+      <c r="X320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -23096,6 +23420,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -23167,6 +23492,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -23242,6 +23568,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -23317,6 +23644,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -23392,6 +23720,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -23463,6 +23792,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -23538,6 +23868,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -23613,6 +23944,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -23684,6 +24016,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -23759,6 +24092,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -23834,6 +24168,7 @@
           <t>Association for Computing Machinery Inc</t>
         </is>
       </c>
+      <c r="X331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -23905,6 +24240,7 @@
           <t>Association for Computing Machinery</t>
         </is>
       </c>
+      <c r="X332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -23976,6 +24312,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -24051,6 +24388,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -24122,6 +24460,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -24197,6 +24536,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -24272,6 +24612,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -24347,6 +24688,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -24422,6 +24764,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -24497,6 +24840,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -24568,6 +24912,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -24643,6 +24988,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -24718,6 +25064,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -24773,6 +25120,7 @@
       <c r="U344" t="inlineStr"/>
       <c r="V344" t="inlineStr"/>
       <c r="W344" t="inlineStr"/>
+      <c r="X344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -24826,6 +25174,7 @@
       <c r="U345" t="inlineStr"/>
       <c r="V345" t="inlineStr"/>
       <c r="W345" t="inlineStr"/>
+      <c r="X345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -24879,6 +25228,7 @@
       <c r="U346" t="inlineStr"/>
       <c r="V346" t="inlineStr"/>
       <c r="W346" t="inlineStr"/>
+      <c r="X346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -24932,6 +25282,7 @@
       <c r="U347" t="inlineStr"/>
       <c r="V347" t="inlineStr"/>
       <c r="W347" t="inlineStr"/>
+      <c r="X347" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -25007,6 +25358,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X348" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -25082,6 +25434,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -25149,6 +25502,7 @@
       <c r="U350" t="inlineStr"/>
       <c r="V350" t="inlineStr"/>
       <c r="W350" t="inlineStr"/>
+      <c r="X350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -25224,6 +25578,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -25295,6 +25650,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -25366,6 +25722,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -25441,6 +25798,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -25512,6 +25870,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -25587,6 +25946,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -25660,6 +26020,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -25735,6 +26096,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -25806,6 +26168,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -25881,6 +26244,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -25948,6 +26312,7 @@
       <c r="U361" t="inlineStr"/>
       <c r="V361" t="inlineStr"/>
       <c r="W361" t="inlineStr"/>
+      <c r="X361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -26023,6 +26388,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -26098,6 +26464,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -26169,6 +26536,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -26244,6 +26612,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -26315,6 +26684,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -26370,6 +26740,7 @@
       <c r="U367" t="inlineStr"/>
       <c r="V367" t="inlineStr"/>
       <c r="W367" t="inlineStr"/>
+      <c r="X367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -26423,6 +26794,7 @@
       <c r="U368" t="inlineStr"/>
       <c r="V368" t="inlineStr"/>
       <c r="W368" t="inlineStr"/>
+      <c r="X368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -26494,6 +26866,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -26569,6 +26942,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -26622,6 +26996,7 @@
       <c r="U371" t="inlineStr"/>
       <c r="V371" t="inlineStr"/>
       <c r="W371" t="inlineStr"/>
+      <c r="X371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -26697,6 +27072,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -26768,6 +27144,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -26827,6 +27204,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -26902,6 +27280,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
@@ -26973,6 +27352,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -27048,6 +27428,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
@@ -27123,6 +27504,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
@@ -27198,6 +27580,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -27273,6 +27656,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
@@ -27344,6 +27728,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
@@ -27397,6 +27782,7 @@
       <c r="U382" t="inlineStr"/>
       <c r="V382" t="inlineStr"/>
       <c r="W382" t="inlineStr"/>
+      <c r="X382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
@@ -27472,6 +27858,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -27543,6 +27930,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X384" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
@@ -27618,6 +28006,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
@@ -27673,6 +28062,7 @@
       <c r="U386" t="inlineStr"/>
       <c r="V386" t="inlineStr"/>
       <c r="W386" t="inlineStr"/>
+      <c r="X386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
@@ -27748,6 +28138,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
@@ -27823,6 +28214,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X388" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
@@ -27898,6 +28290,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X389" t="inlineStr"/>
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
@@ -27963,6 +28356,7 @@
           <t>Institute of Electrical and Electronics Engineers</t>
         </is>
       </c>
+      <c r="X390" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -28016,6 +28410,7 @@
       <c r="U391" t="inlineStr"/>
       <c r="V391" t="inlineStr"/>
       <c r="W391" t="inlineStr"/>
+      <c r="X391" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
@@ -28091,6 +28486,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
@@ -28166,6 +28562,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X393" t="inlineStr"/>
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
@@ -28221,6 +28618,7 @@
       <c r="U394" t="inlineStr"/>
       <c r="V394" t="inlineStr"/>
       <c r="W394" t="inlineStr"/>
+      <c r="X394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
@@ -28292,6 +28690,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X395" t="inlineStr"/>
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
@@ -28347,6 +28746,7 @@
       <c r="U396" t="inlineStr"/>
       <c r="V396" t="inlineStr"/>
       <c r="W396" t="inlineStr"/>
+      <c r="X396" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
@@ -28422,6 +28822,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X397" t="inlineStr"/>
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
@@ -28497,6 +28898,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X398" t="inlineStr"/>
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
@@ -28568,6 +28970,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
@@ -28643,6 +29046,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -28718,6 +29122,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X401" t="inlineStr"/>
     </row>
     <row r="402">
       <c r="A402" s="1" t="n">
@@ -28773,6 +29178,7 @@
       <c r="U402" t="inlineStr"/>
       <c r="V402" t="inlineStr"/>
       <c r="W402" t="inlineStr"/>
+      <c r="X402" t="inlineStr"/>
     </row>
     <row r="403">
       <c r="A403" s="1" t="n">
@@ -28826,6 +29232,7 @@
       <c r="U403" t="inlineStr"/>
       <c r="V403" t="inlineStr"/>
       <c r="W403" t="inlineStr"/>
+      <c r="X403" t="inlineStr"/>
     </row>
     <row r="404">
       <c r="A404" s="1" t="n">
@@ -28901,6 +29308,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X404" t="inlineStr"/>
     </row>
     <row r="405">
       <c r="A405" s="1" t="n">
@@ -28954,6 +29362,7 @@
       <c r="U405" t="inlineStr"/>
       <c r="V405" t="inlineStr"/>
       <c r="W405" t="inlineStr"/>
+      <c r="X405" t="inlineStr"/>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -29007,6 +29416,7 @@
       <c r="U406" t="inlineStr"/>
       <c r="V406" t="inlineStr"/>
       <c r="W406" t="inlineStr"/>
+      <c r="X406" t="inlineStr"/>
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
@@ -29078,6 +29488,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X407" t="inlineStr"/>
     </row>
     <row r="408">
       <c r="A408" s="1" t="n">
@@ -29153,6 +29564,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X408" t="inlineStr"/>
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
@@ -29220,6 +29632,7 @@
       <c r="U409" t="inlineStr"/>
       <c r="V409" t="inlineStr"/>
       <c r="W409" t="inlineStr"/>
+      <c r="X409" t="inlineStr"/>
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
@@ -29295,6 +29708,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X410" t="inlineStr"/>
     </row>
     <row r="411">
       <c r="A411" s="1" t="n">
@@ -29366,6 +29780,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X411" t="inlineStr"/>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -29437,6 +29852,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X412" t="inlineStr"/>
     </row>
     <row r="413">
       <c r="A413" s="1" t="n">
@@ -29490,6 +29906,7 @@
       <c r="U413" t="inlineStr"/>
       <c r="V413" t="inlineStr"/>
       <c r="W413" t="inlineStr"/>
+      <c r="X413" t="inlineStr"/>
     </row>
     <row r="414">
       <c r="A414" s="1" t="n">
@@ -29543,6 +29960,7 @@
       <c r="U414" t="inlineStr"/>
       <c r="V414" t="inlineStr"/>
       <c r="W414" t="inlineStr"/>
+      <c r="X414" t="inlineStr"/>
     </row>
     <row r="415">
       <c r="A415" s="1" t="n">
@@ -29598,6 +30016,7 @@
       <c r="U415" t="inlineStr"/>
       <c r="V415" t="inlineStr"/>
       <c r="W415" t="inlineStr"/>
+      <c r="X415" t="inlineStr"/>
     </row>
     <row r="416">
       <c r="A416" s="1" t="n">
@@ -29673,6 +30092,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X416" t="inlineStr"/>
     </row>
     <row r="417">
       <c r="A417" s="1" t="n">
@@ -29748,6 +30168,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X417" t="inlineStr"/>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -29819,6 +30240,7 @@
           <t>IEEE Computer Society</t>
         </is>
       </c>
+      <c r="X418" t="inlineStr"/>
     </row>
     <row r="419">
       <c r="A419" s="1" t="n">
@@ -29894,6 +30316,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X419" t="inlineStr"/>
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
@@ -29947,6 +30370,7 @@
       <c r="U420" t="inlineStr"/>
       <c r="V420" t="inlineStr"/>
       <c r="W420" t="inlineStr"/>
+      <c r="X420" t="inlineStr"/>
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
@@ -30022,6 +30446,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X421" t="inlineStr"/>
     </row>
     <row r="422">
       <c r="A422" s="1" t="n">
@@ -30097,6 +30522,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X422" t="inlineStr"/>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
@@ -30150,6 +30576,7 @@
       <c r="U423" t="inlineStr"/>
       <c r="V423" t="inlineStr"/>
       <c r="W423" t="inlineStr"/>
+      <c r="X423" t="inlineStr"/>
     </row>
     <row r="424">
       <c r="A424" s="1" t="n">
@@ -30225,6 +30652,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X424" t="inlineStr"/>
     </row>
     <row r="425">
       <c r="A425" s="1" t="n">
@@ -30304,6 +30732,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X425" t="inlineStr"/>
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
@@ -30375,6 +30804,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X426" t="inlineStr"/>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -30450,6 +30880,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X427" t="inlineStr"/>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
@@ -30521,6 +30952,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X428" t="inlineStr"/>
     </row>
     <row r="429">
       <c r="A429" s="1" t="n">
@@ -30596,6 +31028,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X429" t="inlineStr"/>
     </row>
     <row r="430">
       <c r="A430" s="1" t="n">
@@ -30673,6 +31106,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X430" t="inlineStr"/>
     </row>
     <row r="431">
       <c r="A431" s="1" t="n">
@@ -30726,6 +31160,7 @@
       <c r="U431" t="inlineStr"/>
       <c r="V431" t="inlineStr"/>
       <c r="W431" t="inlineStr"/>
+      <c r="X431" t="inlineStr"/>
     </row>
     <row r="432">
       <c r="A432" s="1" t="n">
@@ -30797,6 +31232,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X432" t="inlineStr"/>
     </row>
     <row r="433">
       <c r="A433" s="1" t="n">
@@ -30872,6 +31308,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X433" t="inlineStr"/>
     </row>
     <row r="434">
       <c r="A434" s="1" t="n">
@@ -30943,6 +31380,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X434" t="inlineStr"/>
     </row>
     <row r="435">
       <c r="A435" s="1" t="n">
@@ -31012,6 +31450,7 @@
         </is>
       </c>
       <c r="W435" t="inlineStr"/>
+      <c r="X435" t="inlineStr"/>
     </row>
     <row r="436">
       <c r="A436" s="1" t="n">
@@ -31081,6 +31520,7 @@
         </is>
       </c>
       <c r="W436" t="inlineStr"/>
+      <c r="X436" t="inlineStr"/>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
@@ -31156,6 +31596,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X437" t="inlineStr"/>
     </row>
     <row r="438">
       <c r="A438" s="1" t="n">
@@ -31209,6 +31650,7 @@
       <c r="U438" t="inlineStr"/>
       <c r="V438" t="inlineStr"/>
       <c r="W438" t="inlineStr"/>
+      <c r="X438" t="inlineStr"/>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
@@ -31282,6 +31724,7 @@
           <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
         </is>
       </c>
+      <c r="X439" t="inlineStr"/>
     </row>
     <row r="440">
       <c r="A440" s="1" t="n">
@@ -31335,6 +31778,7 @@
       <c r="U440" t="inlineStr"/>
       <c r="V440" t="inlineStr"/>
       <c r="W440" t="inlineStr"/>
+      <c r="X440" t="inlineStr"/>
     </row>
     <row r="441">
       <c r="A441" s="1" t="n">
@@ -31406,6 +31850,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X441" t="inlineStr"/>
     </row>
     <row r="442">
       <c r="A442" s="1" t="n">
@@ -31481,6 +31926,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X442" t="inlineStr"/>
     </row>
     <row r="443">
       <c r="A443" s="1" t="n">
@@ -31556,6 +32002,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X443" t="inlineStr"/>
     </row>
     <row r="444">
       <c r="A444" s="1" t="n">
@@ -31611,6 +32058,7 @@
       <c r="U444" t="inlineStr"/>
       <c r="V444" t="inlineStr"/>
       <c r="W444" t="inlineStr"/>
+      <c r="X444" t="inlineStr"/>
     </row>
     <row r="445">
       <c r="A445" s="1" t="n">
@@ -31686,6 +32134,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X445" t="inlineStr"/>
     </row>
     <row r="446">
       <c r="A446" s="1" t="n">
@@ -31761,6 +32210,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X446" t="inlineStr"/>
     </row>
     <row r="447">
       <c r="A447" s="1" t="n">
@@ -31836,6 +32286,7 @@
           <t>IEEE</t>
         </is>
       </c>
+      <c r="X447" t="inlineStr"/>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
@@ -31911,6 +32362,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X448" t="inlineStr"/>
     </row>
     <row r="449">
       <c r="A449" s="1" t="n">
@@ -31986,6 +32438,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X449" t="inlineStr"/>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
@@ -32039,6 +32492,7 @@
       <c r="U450" t="inlineStr"/>
       <c r="V450" t="inlineStr"/>
       <c r="W450" t="inlineStr"/>
+      <c r="X450" t="inlineStr"/>
     </row>
     <row r="451">
       <c r="A451" s="1" t="n">
@@ -32092,6 +32546,7 @@
       <c r="U451" t="inlineStr"/>
       <c r="V451" t="inlineStr"/>
       <c r="W451" t="inlineStr"/>
+      <c r="X451" t="inlineStr"/>
     </row>
     <row r="452">
       <c r="A452" s="1" t="n">
@@ -32163,6 +32618,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X452" t="inlineStr"/>
     </row>
     <row r="453">
       <c r="A453" s="1" t="n">
@@ -32218,6 +32674,7 @@
       <c r="U453" t="inlineStr"/>
       <c r="V453" t="inlineStr"/>
       <c r="W453" t="inlineStr"/>
+      <c r="X453" t="inlineStr"/>
     </row>
     <row r="454">
       <c r="A454" s="1" t="n">
@@ -32293,6 +32750,7 @@
           <t>Institute of Electrical and Electronics Engineers Inc.</t>
         </is>
       </c>
+      <c r="X454" t="inlineStr"/>
     </row>
     <row r="455">
       <c r="A455" s="1" t="n">
@@ -32364,6 +32822,7 @@
           <t>Elsevier B.V.</t>
         </is>
       </c>
+      <c r="X455" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>